<commit_message>
added statistic analysis from different technologies and plot
</commit_message>
<xml_diff>
--- a/ExtractedData/HeuristicData/pypdf2/spacy/KeywordFrequency/keyword_validation.xlsx
+++ b/ExtractedData/HeuristicData/pypdf2/spacy/KeywordFrequency/keyword_validation.xlsx
@@ -1703,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="AH2">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:34">
@@ -1807,7 +1807,7 @@
         <v>2</v>
       </c>
       <c r="AH3">
-        <v>1625</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -1911,7 +1911,7 @@
         <v>0</v>
       </c>
       <c r="AH4">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:34">
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="AH5">
-        <v>120</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:34">
@@ -2327,7 +2327,7 @@
         <v>20</v>
       </c>
       <c r="AH8">
-        <v>3430</v>
+        <v>7546</v>
       </c>
     </row>
     <row r="9" spans="1:34">
@@ -2431,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="AH9">
-        <v>1810</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="10" spans="1:34">
@@ -2535,7 +2535,7 @@
         <v>2</v>
       </c>
       <c r="AH10">
-        <v>1480</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="11" spans="1:34">
@@ -2639,7 +2639,7 @@
         <v>0</v>
       </c>
       <c r="AH11">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:34">
@@ -2951,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:34">
@@ -3055,7 +3055,7 @@
         <v>64</v>
       </c>
       <c r="AH15">
-        <v>12500</v>
+        <v>27500</v>
       </c>
     </row>
     <row r="16" spans="1:34">
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="AH16">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:34">
@@ -3263,7 +3263,7 @@
         <v>11</v>
       </c>
       <c r="AH17">
-        <v>695</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="18" spans="1:34">
@@ -3575,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="AH20">
-        <v>80</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:34">
@@ -3783,7 +3783,7 @@
         <v>64</v>
       </c>
       <c r="AH22">
-        <v>4580</v>
+        <v>10076</v>
       </c>
     </row>
     <row r="23" spans="1:34">
@@ -3887,7 +3887,7 @@
         <v>0</v>
       </c>
       <c r="AH23">
-        <v>105</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:34">
@@ -3991,7 +3991,7 @@
         <v>68</v>
       </c>
       <c r="AH24">
-        <v>4645</v>
+        <v>10219</v>
       </c>
     </row>
     <row r="25" spans="1:34">
@@ -4095,7 +4095,7 @@
         <v>0</v>
       </c>
       <c r="AH25">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:34">
@@ -4199,7 +4199,7 @@
         <v>6</v>
       </c>
       <c r="AH26">
-        <v>55</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:34">
@@ -4303,7 +4303,7 @@
         <v>27</v>
       </c>
       <c r="AH27">
-        <v>1215</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="28" spans="1:34">
@@ -4407,7 +4407,7 @@
         <v>81</v>
       </c>
       <c r="AH28">
-        <v>15380</v>
+        <v>33836</v>
       </c>
     </row>
     <row r="29" spans="1:34">
@@ -4511,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="AH29">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:34">
@@ -4719,7 +4719,7 @@
         <v>0</v>
       </c>
       <c r="AH31">
-        <v>435</v>
+        <v>957</v>
       </c>
     </row>
     <row r="32" spans="1:34">
@@ -4823,7 +4823,7 @@
         <v>43</v>
       </c>
       <c r="AH32">
-        <v>13810</v>
+        <v>30382</v>
       </c>
     </row>
     <row r="33" spans="1:34">
@@ -4927,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="AH33">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:34">
@@ -5031,7 +5031,7 @@
         <v>16</v>
       </c>
       <c r="AH34">
-        <v>4840</v>
+        <v>10648</v>
       </c>
     </row>
     <row r="35" spans="1:34">
@@ -5239,7 +5239,7 @@
         <v>65</v>
       </c>
       <c r="AH36">
-        <v>17970</v>
+        <v>39534</v>
       </c>
     </row>
     <row r="37" spans="1:34">
@@ -5655,7 +5655,7 @@
         <v>0</v>
       </c>
       <c r="AH40">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:34">
@@ -5759,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="AH41">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:34">
@@ -5863,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="AH42">
-        <v>805</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="43" spans="1:34">
@@ -5967,7 +5967,7 @@
         <v>4</v>
       </c>
       <c r="AH43">
-        <v>750</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="44" spans="1:34">
@@ -6071,7 +6071,7 @@
         <v>1</v>
       </c>
       <c r="AH44">
-        <v>595</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="45" spans="1:34">
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="AH45">
-        <v>150</v>
+        <v>330</v>
       </c>
     </row>
     <row r="46" spans="1:34">
@@ -6383,7 +6383,7 @@
         <v>0</v>
       </c>
       <c r="AH47">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:34">
@@ -6695,7 +6695,7 @@
         <v>0</v>
       </c>
       <c r="AH50">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:34">
@@ -7423,7 +7423,7 @@
         <v>0</v>
       </c>
       <c r="AH57">
-        <v>1900</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="58" spans="1:34">
@@ -7527,7 +7527,7 @@
         <v>78</v>
       </c>
       <c r="AH58">
-        <v>9310</v>
+        <v>20482</v>
       </c>
     </row>
     <row r="59" spans="1:34">
@@ -8047,7 +8047,7 @@
         <v>0</v>
       </c>
       <c r="AH63">
-        <v>865</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="64" spans="1:34">
@@ -8151,7 +8151,7 @@
         <v>1</v>
       </c>
       <c r="AH64">
-        <v>1680</v>
+        <v>3696</v>
       </c>
     </row>
     <row r="65" spans="1:34">
@@ -8359,7 +8359,7 @@
         <v>0</v>
       </c>
       <c r="AH66">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:34">
@@ -8671,7 +8671,7 @@
         <v>0</v>
       </c>
       <c r="AH69">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:34">
@@ -8983,7 +8983,7 @@
         <v>0</v>
       </c>
       <c r="AH72">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:34">
@@ -10335,7 +10335,7 @@
         <v>0</v>
       </c>
       <c r="AH85">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:34">
@@ -10751,7 +10751,7 @@
         <v>0</v>
       </c>
       <c r="AH89">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:34">
@@ -10855,7 +10855,7 @@
         <v>0</v>
       </c>
       <c r="AH90">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="1:34">
@@ -10959,7 +10959,7 @@
         <v>0</v>
       </c>
       <c r="AH91">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:34">
@@ -11063,7 +11063,7 @@
         <v>0</v>
       </c>
       <c r="AH92">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:34">
@@ -11167,7 +11167,7 @@
         <v>0</v>
       </c>
       <c r="AH93">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:34">
@@ -11271,7 +11271,7 @@
         <v>0</v>
       </c>
       <c r="AH94">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:34">
@@ -11375,7 +11375,7 @@
         <v>1</v>
       </c>
       <c r="AH95">
-        <v>395</v>
+        <v>869</v>
       </c>
     </row>
     <row r="96" spans="1:34">
@@ -11479,7 +11479,7 @@
         <v>1</v>
       </c>
       <c r="AH96">
-        <v>135</v>
+        <v>297</v>
       </c>
     </row>
     <row r="97" spans="1:34">
@@ -11583,7 +11583,7 @@
         <v>0</v>
       </c>
       <c r="AH97">
-        <v>95</v>
+        <v>209</v>
       </c>
     </row>
     <row r="98" spans="1:34">
@@ -11687,7 +11687,7 @@
         <v>0</v>
       </c>
       <c r="AH98">
-        <v>245</v>
+        <v>539</v>
       </c>
     </row>
     <row r="99" spans="1:34">
@@ -11895,7 +11895,7 @@
         <v>0</v>
       </c>
       <c r="AH100">
-        <v>175</v>
+        <v>385</v>
       </c>
     </row>
     <row r="101" spans="1:34">
@@ -12103,7 +12103,7 @@
         <v>20</v>
       </c>
       <c r="AH102">
-        <v>3575</v>
+        <v>7865</v>
       </c>
     </row>
     <row r="103" spans="1:34">
@@ -12207,7 +12207,7 @@
         <v>0</v>
       </c>
       <c r="AH103">
-        <v>65</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:34">
@@ -12311,7 +12311,7 @@
         <v>0</v>
       </c>
       <c r="AH104">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:34">
@@ -12415,7 +12415,7 @@
         <v>0</v>
       </c>
       <c r="AH105">
-        <v>325</v>
+        <v>715</v>
       </c>
     </row>
     <row r="106" spans="1:34">
@@ -12727,7 +12727,7 @@
         <v>2</v>
       </c>
       <c r="AH108">
-        <v>200</v>
+        <v>440</v>
       </c>
     </row>
     <row r="109" spans="1:34">
@@ -12831,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="AH109">
-        <v>185</v>
+        <v>407</v>
       </c>
     </row>
     <row r="110" spans="1:34">
@@ -12935,7 +12935,7 @@
         <v>0</v>
       </c>
       <c r="AH110">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111" spans="1:34">
@@ -13039,7 +13039,7 @@
         <v>0</v>
       </c>
       <c r="AH111">
-        <v>385</v>
+        <v>847</v>
       </c>
     </row>
     <row r="112" spans="1:34">
@@ -13351,7 +13351,7 @@
         <v>0</v>
       </c>
       <c r="AH114">
-        <v>15755</v>
+        <v>34661</v>
       </c>
     </row>
     <row r="115" spans="1:34">
@@ -13767,7 +13767,7 @@
         <v>0</v>
       </c>
       <c r="AH118">
-        <v>1810</v>
+        <v>3982</v>
       </c>
     </row>
     <row r="119" spans="1:34">
@@ -13871,7 +13871,7 @@
         <v>0</v>
       </c>
       <c r="AH119">
-        <v>330</v>
+        <v>726</v>
       </c>
     </row>
     <row r="120" spans="1:34">
@@ -13975,7 +13975,7 @@
         <v>0</v>
       </c>
       <c r="AH120">
-        <v>465</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="121" spans="1:34">
@@ -14079,7 +14079,7 @@
         <v>0</v>
       </c>
       <c r="AH121">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:34">
@@ -14287,7 +14287,7 @@
         <v>0</v>
       </c>
       <c r="AH123">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="124" spans="1:34">
@@ -14703,7 +14703,7 @@
         <v>0</v>
       </c>
       <c r="AH127">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128" spans="1:34">
@@ -14911,7 +14911,7 @@
         <v>0</v>
       </c>
       <c r="AH129">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="130" spans="1:34">
@@ -15951,7 +15951,7 @@
         <v>0</v>
       </c>
       <c r="AH139">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="140" spans="1:34">
@@ -16055,7 +16055,7 @@
         <v>0</v>
       </c>
       <c r="AH140">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="141" spans="1:34">
@@ -16367,7 +16367,7 @@
         <v>0</v>
       </c>
       <c r="AH143">
-        <v>35</v>
+        <v>77</v>
       </c>
     </row>
     <row r="144" spans="1:34">
@@ -16471,7 +16471,7 @@
         <v>0</v>
       </c>
       <c r="AH144">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145" spans="1:34">
@@ -16679,7 +16679,7 @@
         <v>32</v>
       </c>
       <c r="AH146">
-        <v>1150</v>
+        <v>2530</v>
       </c>
     </row>
     <row r="147" spans="1:34">
@@ -16991,7 +16991,7 @@
         <v>0</v>
       </c>
       <c r="AH149">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="150" spans="1:34">
@@ -17927,7 +17927,7 @@
         <v>0</v>
       </c>
       <c r="AH158">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="159" spans="1:34">
@@ -18031,7 +18031,7 @@
         <v>4</v>
       </c>
       <c r="AH159">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="160" spans="1:34">
@@ -18447,7 +18447,7 @@
         <v>0</v>
       </c>
       <c r="AH163">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="164" spans="1:34">
@@ -18863,7 +18863,7 @@
         <v>0</v>
       </c>
       <c r="AH167">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="168" spans="1:34">
@@ -18967,7 +18967,7 @@
         <v>0</v>
       </c>
       <c r="AH168">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="169" spans="1:34">
@@ -19071,7 +19071,7 @@
         <v>0</v>
       </c>
       <c r="AH169">
-        <v>650</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="170" spans="1:34">
@@ -19175,7 +19175,7 @@
         <v>0</v>
       </c>
       <c r="AH170">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:34">
@@ -19383,7 +19383,7 @@
         <v>0</v>
       </c>
       <c r="AH172">
-        <v>435</v>
+        <v>957</v>
       </c>
     </row>
     <row r="173" spans="1:34">
@@ -20007,7 +20007,7 @@
         <v>0</v>
       </c>
       <c r="AH178">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:34">
@@ -20631,7 +20631,7 @@
         <v>0</v>
       </c>
       <c r="AH184">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:34">
@@ -21359,7 +21359,7 @@
         <v>0</v>
       </c>
       <c r="AH191">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="192" spans="1:34">
@@ -21775,7 +21775,7 @@
         <v>0</v>
       </c>
       <c r="AH195">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="196" spans="1:34">
@@ -23023,7 +23023,7 @@
         <v>0</v>
       </c>
       <c r="AH207">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="208" spans="1:34">
@@ -23335,7 +23335,7 @@
         <v>0</v>
       </c>
       <c r="AH210">
-        <v>60</v>
+        <v>132</v>
       </c>
     </row>
     <row r="211" spans="1:34">
@@ -25311,7 +25311,7 @@
         <v>0</v>
       </c>
       <c r="AH229">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="230" spans="1:34">
@@ -26559,7 +26559,7 @@
         <v>0</v>
       </c>
       <c r="AH241">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="242" spans="1:34">
@@ -26767,7 +26767,7 @@
         <v>44</v>
       </c>
       <c r="AH243">
-        <v>9005</v>
+        <v>19811</v>
       </c>
     </row>
     <row r="244" spans="1:34">
@@ -26871,7 +26871,7 @@
         <v>0</v>
       </c>
       <c r="AH244">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="245" spans="1:34">
@@ -26975,7 +26975,7 @@
         <v>0</v>
       </c>
       <c r="AH245">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="246" spans="1:34">
@@ -27079,7 +27079,7 @@
         <v>0</v>
       </c>
       <c r="AH246">
-        <v>900</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="247" spans="1:34">
@@ -27287,7 +27287,7 @@
         <v>1</v>
       </c>
       <c r="AH248">
-        <v>5665</v>
+        <v>12463</v>
       </c>
     </row>
     <row r="249" spans="1:34">
@@ -27391,7 +27391,7 @@
         <v>72</v>
       </c>
       <c r="AH249">
-        <v>27630</v>
+        <v>60786</v>
       </c>
     </row>
     <row r="250" spans="1:34">
@@ -27495,7 +27495,7 @@
         <v>3</v>
       </c>
       <c r="AH250">
-        <v>950</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="251" spans="1:34">
@@ -27599,7 +27599,7 @@
         <v>0</v>
       </c>
       <c r="AH251">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="252" spans="1:34">
@@ -27807,7 +27807,7 @@
         <v>13</v>
       </c>
       <c r="AH253">
-        <v>460</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="254" spans="1:34">
@@ -28015,7 +28015,7 @@
         <v>0</v>
       </c>
       <c r="AH255">
-        <v>145</v>
+        <v>319</v>
       </c>
     </row>
     <row r="256" spans="1:34">
@@ -28223,7 +28223,7 @@
         <v>0</v>
       </c>
       <c r="AH257">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="258" spans="1:34">
@@ -28639,7 +28639,7 @@
         <v>0</v>
       </c>
       <c r="AH261">
-        <v>290</v>
+        <v>638</v>
       </c>
     </row>
     <row r="262" spans="1:34">
@@ -29471,7 +29471,7 @@
         <v>0</v>
       </c>
       <c r="AH269">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="270" spans="1:34">
@@ -29679,7 +29679,7 @@
         <v>0</v>
       </c>
       <c r="AH271">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="272" spans="1:34">
@@ -30199,7 +30199,7 @@
         <v>0</v>
       </c>
       <c r="AH276">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="277" spans="1:34">
@@ -30303,7 +30303,7 @@
         <v>2</v>
       </c>
       <c r="AH277">
-        <v>930</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="278" spans="1:34">
@@ -30407,7 +30407,7 @@
         <v>0</v>
       </c>
       <c r="AH278">
-        <v>740</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="279" spans="1:34">
@@ -30511,7 +30511,7 @@
         <v>0</v>
       </c>
       <c r="AH279">
-        <v>2360</v>
+        <v>5192</v>
       </c>
     </row>
     <row r="280" spans="1:34">
@@ -30615,7 +30615,7 @@
         <v>16</v>
       </c>
       <c r="AH280">
-        <v>8670</v>
+        <v>19074</v>
       </c>
     </row>
     <row r="281" spans="1:34">
@@ -30719,7 +30719,7 @@
         <v>5</v>
       </c>
       <c r="AH281">
-        <v>310</v>
+        <v>682</v>
       </c>
     </row>
     <row r="282" spans="1:34">
@@ -30823,7 +30823,7 @@
         <v>0</v>
       </c>
       <c r="AH282">
-        <v>190</v>
+        <v>418</v>
       </c>
     </row>
     <row r="283" spans="1:34">
@@ -31031,7 +31031,7 @@
         <v>0</v>
       </c>
       <c r="AH284">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="285" spans="1:34">
@@ -31135,7 +31135,7 @@
         <v>0</v>
       </c>
       <c r="AH285">
-        <v>195</v>
+        <v>429</v>
       </c>
     </row>
     <row r="286" spans="1:34">
@@ -31239,7 +31239,7 @@
         <v>1</v>
       </c>
       <c r="AH286">
-        <v>395</v>
+        <v>869</v>
       </c>
     </row>
     <row r="287" spans="1:34">
@@ -31343,7 +31343,7 @@
         <v>27</v>
       </c>
       <c r="AH287">
-        <v>15970</v>
+        <v>35134</v>
       </c>
     </row>
     <row r="288" spans="1:34">
@@ -31551,7 +31551,7 @@
         <v>0</v>
       </c>
       <c r="AH289">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="290" spans="1:34">
@@ -31759,7 +31759,7 @@
         <v>0</v>
       </c>
       <c r="AH291">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="292" spans="1:34">
@@ -32175,7 +32175,7 @@
         <v>0</v>
       </c>
       <c r="AH295">
-        <v>60</v>
+        <v>132</v>
       </c>
     </row>
     <row r="296" spans="1:34">
@@ -32279,7 +32279,7 @@
         <v>0</v>
       </c>
       <c r="AH296">
-        <v>730</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="297" spans="1:34">
@@ -32383,7 +32383,7 @@
         <v>1</v>
       </c>
       <c r="AH297">
-        <v>625</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="298" spans="1:34">
@@ -32487,7 +32487,7 @@
         <v>0</v>
       </c>
       <c r="AH298">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="299" spans="1:34">
@@ -32903,7 +32903,7 @@
         <v>0</v>
       </c>
       <c r="AH302">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="303" spans="1:34">
@@ -33007,7 +33007,7 @@
         <v>0</v>
       </c>
       <c r="AH303">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="304" spans="1:34">
@@ -33319,7 +33319,7 @@
         <v>0</v>
       </c>
       <c r="AH306">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="307" spans="1:34">
@@ -33527,7 +33527,7 @@
         <v>0</v>
       </c>
       <c r="AH308">
-        <v>360</v>
+        <v>792</v>
       </c>
     </row>
     <row r="309" spans="1:34">
@@ -33631,7 +33631,7 @@
         <v>0</v>
       </c>
       <c r="AH309">
-        <v>595</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="310" spans="1:34">
@@ -33839,7 +33839,7 @@
         <v>0</v>
       </c>
       <c r="AH311">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="312" spans="1:34">
@@ -34255,7 +34255,7 @@
         <v>0</v>
       </c>
       <c r="AH315">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="316" spans="1:34">
@@ -35191,7 +35191,7 @@
         <v>0</v>
       </c>
       <c r="AH324">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="325" spans="1:34">
@@ -35711,7 +35711,7 @@
         <v>0</v>
       </c>
       <c r="AH329">
-        <v>1055</v>
+        <v>2321</v>
       </c>
     </row>
     <row r="330" spans="1:34">
@@ -35815,7 +35815,7 @@
         <v>0</v>
       </c>
       <c r="AH330">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="331" spans="1:34">
@@ -35919,7 +35919,7 @@
         <v>6</v>
       </c>
       <c r="AH331">
-        <v>2290</v>
+        <v>5038</v>
       </c>
     </row>
   </sheetData>

</xml_diff>